<commit_message>
Change structure of action charter like action sell.
</commit_message>
<xml_diff>
--- a/output/ship_rule_integrate.xlsx
+++ b/output/ship_rule_integrate.xlsx
@@ -383,33 +383,35 @@
         </is>
       </c>
       <c r="B1" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>24</v>
+        <v>650</v>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="0" t="n">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>5</v>
@@ -417,29 +419,29 @@
     </row>
     <row r="3">
       <c r="B3" s="0" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>900</v>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2712599465697811</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -449,33 +451,35 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>24</v>
+        <v>650</v>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="0" t="n">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1500</v>
+        <v>1100</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>5</v>
@@ -483,29 +487,29 @@
     </row>
     <row r="7">
       <c r="B7" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>900</v>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2712599465697811</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -515,33 +519,35 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>24</v>
+        <v>650</v>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="0" t="n">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>5</v>
@@ -549,29 +555,29 @@
     </row>
     <row r="11">
       <c r="B11" s="0" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>900</v>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2712599465697811</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -581,27 +587,29 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>24</v>
+        <v>750</v>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
@@ -615,29 +623,29 @@
     </row>
     <row r="15">
       <c r="B15" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2712599465697811</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -647,27 +655,29 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>24</v>
+        <v>750</v>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0</v>
@@ -681,29 +691,29 @@
     </row>
     <row r="19">
       <c r="B19" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2712599465697811</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -713,33 +723,35 @@
         </is>
       </c>
       <c r="B21" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>24</v>
+        <v>650</v>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="0" t="n">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>5</v>
@@ -747,29 +759,29 @@
     </row>
     <row r="23">
       <c r="B23" s="0" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>900</v>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2712599465697811</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -779,33 +791,35 @@
         </is>
       </c>
       <c r="B25" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>24</v>
+        <v>650</v>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="0" t="n">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>5</v>
@@ -813,29 +827,29 @@
     </row>
     <row r="27">
       <c r="B27" s="0" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>900</v>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2712599465697811</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -845,30 +859,30 @@
         </is>
       </c>
       <c r="B29" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>700</v>
@@ -879,29 +893,29 @@
     </row>
     <row r="31">
       <c r="B31" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>400</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>800</v>
+        <v>650</v>
       </c>
       <c r="F31" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2341175254873873</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -911,30 +925,30 @@
         </is>
       </c>
       <c r="B33" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>700</v>
@@ -945,29 +959,29 @@
     </row>
     <row r="35">
       <c r="B35" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>400</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>900</v>
+        <v>650</v>
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2341175254873873</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -977,30 +991,30 @@
         </is>
       </c>
       <c r="B37" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>700</v>
@@ -1011,29 +1025,29 @@
     </row>
     <row r="39">
       <c r="B39" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>400</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>800</v>
+        <v>650</v>
       </c>
       <c r="F39" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2341175254873873</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1043,30 +1057,30 @@
         </is>
       </c>
       <c r="B41" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>700</v>
@@ -1077,29 +1091,29 @@
     </row>
     <row r="43">
       <c r="B43" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>400</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>900</v>
+        <v>650</v>
       </c>
       <c r="F43" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2341175254873873</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1109,30 +1123,30 @@
         </is>
       </c>
       <c r="B45" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>700</v>
@@ -1143,29 +1157,29 @@
     </row>
     <row r="47">
       <c r="B47" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>400</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>900</v>
+        <v>650</v>
       </c>
       <c r="F47" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2341175254873873</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1175,27 +1189,29 @@
         </is>
       </c>
       <c r="B49" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>90</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <v>24</v>
+        <v>750</v>
+      </c>
+      <c r="F49" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>0</v>
@@ -1204,34 +1220,34 @@
         <v>700</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="F51" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2323942347116087</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1241,27 +1257,29 @@
         </is>
       </c>
       <c r="B53" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>90</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>24</v>
+        <v>750</v>
+      </c>
+      <c r="F53" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="B54" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>0</v>
@@ -1270,34 +1288,34 @@
         <v>700</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="F55" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2323942347116087</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1307,27 +1325,29 @@
         </is>
       </c>
       <c r="B57" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>90</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F57" s="0" t="n">
-        <v>24</v>
+        <v>750</v>
+      </c>
+      <c r="F57" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>0</v>
@@ -1336,34 +1356,34 @@
         <v>700</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="F59" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="B60" s="0" t="n">
-        <v>0.2980151311186645</v>
+        <v>0.2323942347116087</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>0.02414928727331264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1373,16 +1393,16 @@
         </is>
       </c>
       <c r="B61" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>90</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F61" s="0" t="inlineStr">
         <is>
@@ -1392,7 +1412,7 @@
     </row>
     <row r="62">
       <c r="B62" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>120</v>
@@ -1401,37 +1421,37 @@
         <v>0</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>1500</v>
       </c>
       <c r="F63" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="B64" s="0" t="n">
-        <v>0.2979315677028281</v>
+        <v>0.2323942347116087</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>0.02412332267807642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1441,16 +1461,16 @@
         </is>
       </c>
       <c r="B65" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>90</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F65" s="0" t="inlineStr">
         <is>
@@ -1460,7 +1480,7 @@
     </row>
     <row r="66">
       <c r="B66" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>120</v>
@@ -1469,37 +1489,37 @@
         <v>0</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>1500</v>
       </c>
       <c r="F67" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="B68" s="0" t="n">
-        <v>0.2979315677028281</v>
+        <v>0.2323942347116087</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>0.02412332267807642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1509,16 +1529,16 @@
         </is>
       </c>
       <c r="B69" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F69" s="0" t="inlineStr">
         <is>
@@ -1528,46 +1548,46 @@
     </row>
     <row r="70">
       <c r="B70" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>1500</v>
+        <v>650</v>
       </c>
       <c r="F71" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>3month charter, 80 ships</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="B72" s="0" t="n">
-        <v>0.2979315677028281</v>
+        <v>0.2279931938282984</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>0.02412332267807642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1577,63 +1597,65 @@
         </is>
       </c>
       <c r="B73" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>24</v>
+        <v>750</v>
+      </c>
+      <c r="F73" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="B74" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>1500</v>
+        <v>650</v>
       </c>
       <c r="F75" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>3month charter, 80 ships</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="B76" s="0" t="n">
-        <v>0.2979315677028281</v>
+        <v>0.2279931938282984</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>0.02412332267807642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1643,65 +1665,63 @@
         </is>
       </c>
       <c r="B77" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F77" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>600</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E78" s="0" t="n">
-        <v>650</v>
+        <v>1000</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="F79" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="B80" s="0" t="n">
-        <v>0.2979315677028281</v>
+        <v>0.2268709139798813</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>0.02412332267807642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1711,65 +1731,63 @@
         </is>
       </c>
       <c r="B81" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F81" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>600</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E82" s="0" t="n">
-        <v>650</v>
+        <v>1000</v>
       </c>
       <c r="F82" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="F83" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="B84" s="0" t="n">
-        <v>0.2979315677028281</v>
+        <v>0.2268709139798813</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>0.02412332267807642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -1779,16 +1797,16 @@
         </is>
       </c>
       <c r="B85" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>600</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F85" s="0" t="inlineStr">
         <is>
@@ -1798,46 +1816,48 @@
     </row>
     <row r="86">
       <c r="B86" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="F86" s="0" t="n">
-        <v>5</v>
+      <c r="F86" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="87">
       <c r="B87" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>400</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="F87" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter, 90 ships</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="B88" s="0" t="n">
-        <v>0.2694056624996978</v>
+        <v>-0.4695675081548457</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>0.0160759426899423</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1847,63 +1867,67 @@
         </is>
       </c>
       <c r="B89" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F89" s="0" t="n">
-        <v>24</v>
+        <v>750</v>
+      </c>
+      <c r="F89" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="90">
       <c r="B90" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E90" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="F90" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F90" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="91">
       <c r="B91" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="F91" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>3month charter, 90 ships</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="B92" s="0" t="n">
-        <v>0.2694056624996978</v>
+        <v>-0.4695675081548457</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>0.0160759426899423</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -1913,16 +1937,16 @@
         </is>
       </c>
       <c r="B93" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F93" s="0" t="inlineStr">
         <is>
@@ -1932,10 +1956,10 @@
     </row>
     <row r="94">
       <c r="B94" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>0</v>
@@ -1943,35 +1967,37 @@
       <c r="E94" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="F94" s="0" t="n">
-        <v>5</v>
+      <c r="F94" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="95">
       <c r="B95" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="F95" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="B96" s="0" t="n">
-        <v>0.2694056624996978</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>0.0160759426899423</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -1981,16 +2007,16 @@
         </is>
       </c>
       <c r="B97" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D97" s="0" t="n">
         <v>550</v>
       </c>
       <c r="E97" s="0" t="n">
-        <v>1300</v>
+        <v>750</v>
       </c>
       <c r="F97" s="0" t="inlineStr">
         <is>
@@ -2000,46 +2026,48 @@
     </row>
     <row r="98">
       <c r="B98" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E98" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F98" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F98" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="99">
       <c r="B99" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E99" s="0" t="n">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="F99" s="0" t="inlineStr">
         <is>
-          <t>36month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="B100" s="0" t="n">
-        <v>0.2694056624996978</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>0.0160759426899423</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -2049,50 +2077,54 @@
         </is>
       </c>
       <c r="B101" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C101" s="0" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="D101" s="0" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>750</v>
       </c>
-      <c r="F101" s="0" t="n">
-        <v>24</v>
+      <c r="F101" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="102">
       <c r="B102" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E102" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F102" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F102" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="103">
       <c r="B103" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C103" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="C103" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="D103" s="0" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="E103" s="0" t="n">
-        <v>1500</v>
+        <v>650</v>
       </c>
       <c r="F103" s="0" t="inlineStr">
         <is>
@@ -2102,10 +2134,10 @@
     </row>
     <row r="104">
       <c r="B104" s="0" t="n">
-        <v>0.2455460155721056</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C104" s="0" t="n">
-        <v>0.01059485127529065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -2115,16 +2147,16 @@
         </is>
       </c>
       <c r="B105" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C105" s="0" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E105" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F105" s="0" t="inlineStr">
         <is>
@@ -2134,33 +2166,35 @@
     </row>
     <row r="106">
       <c r="B106" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C106" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D106" s="0" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="F106" s="0" t="n">
-        <v>5</v>
+      <c r="F106" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="107">
       <c r="B107" s="0" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C107" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D107" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E107" s="0" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="F107" s="0" t="inlineStr">
         <is>
@@ -2170,10 +2204,10 @@
     </row>
     <row r="108">
       <c r="B108" s="0" t="n">
-        <v>0.2455460155721056</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C108" s="0" t="n">
-        <v>0.01059485127529065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -2183,16 +2217,16 @@
         </is>
       </c>
       <c r="B109" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C109" s="0" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E109" s="0" t="n">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="F109" s="0" t="inlineStr">
         <is>
@@ -2202,33 +2236,35 @@
     </row>
     <row r="110">
       <c r="B110" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C110" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="F110" s="0" t="n">
-        <v>5</v>
+      <c r="F110" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="111">
       <c r="B111" s="0" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C111" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E111" s="0" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="F111" s="0" t="inlineStr">
         <is>
@@ -2238,10 +2274,10 @@
     </row>
     <row r="112">
       <c r="B112" s="0" t="n">
-        <v>0.2455460155721056</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>0.01059485127529065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -2251,16 +2287,16 @@
         </is>
       </c>
       <c r="B113" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C113" s="0" t="n">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="D113" s="0" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="E113" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F113" s="0" t="inlineStr">
         <is>
@@ -2270,33 +2306,35 @@
     </row>
     <row r="114">
       <c r="B114" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C114" s="0" t="n">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D114" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E114" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F114" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F114" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="115">
       <c r="B115" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C115" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="E115" s="0" t="n">
-        <v>900</v>
+        <v>650</v>
       </c>
       <c r="F115" s="0" t="inlineStr">
         <is>
@@ -2306,10 +2344,10 @@
     </row>
     <row r="116">
       <c r="B116" s="0" t="n">
-        <v>0.2455460155721056</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C116" s="0" t="n">
-        <v>0.01059485127529065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -2319,50 +2357,54 @@
         </is>
       </c>
       <c r="B117" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C117" s="0" t="n">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E117" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="F117" s="0" t="n">
-        <v>24</v>
+        <v>700</v>
+      </c>
+      <c r="F117" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="118">
       <c r="B118" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C118" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D118" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E118" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F118" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F118" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="119">
       <c r="B119" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C119" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D119" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E119" s="0" t="n">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="F119" s="0" t="inlineStr">
         <is>
@@ -2372,10 +2414,10 @@
     </row>
     <row r="120">
       <c r="B120" s="0" t="n">
-        <v>0.2455460155721056</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C120" s="0" t="n">
-        <v>0.01059485127529065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -2385,16 +2427,16 @@
         </is>
       </c>
       <c r="B121" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C121" s="0" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="D121" s="0" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E121" s="0" t="n">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="F121" s="0" t="inlineStr">
         <is>
@@ -2404,33 +2446,35 @@
     </row>
     <row r="122">
       <c r="B122" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C122" s="0" t="n">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D122" s="0" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E122" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="F122" s="0" t="n">
-        <v>5</v>
+      <c r="F122" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="123">
       <c r="B123" s="0" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C123" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D123" s="0" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="E123" s="0" t="n">
-        <v>900</v>
+        <v>650</v>
       </c>
       <c r="F123" s="0" t="inlineStr">
         <is>
@@ -2440,10 +2484,10 @@
     </row>
     <row r="124">
       <c r="B124" s="0" t="n">
-        <v>0.2455460155721056</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C124" s="0" t="n">
-        <v>0.01059485127529065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -2453,63 +2497,67 @@
         </is>
       </c>
       <c r="B125" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C125" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D125" s="0" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="E125" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="F125" s="0" t="n">
-        <v>19</v>
+        <v>750</v>
+      </c>
+      <c r="F125" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="126">
       <c r="B126" s="0" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C126" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D126" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E126" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F126" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F126" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="127">
       <c r="B127" s="0" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D127" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="F127" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="B128" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C128" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -2519,16 +2567,16 @@
         </is>
       </c>
       <c r="B129" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C129" s="0" t="n">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="D129" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E129" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="F129" s="0" t="inlineStr">
         <is>
@@ -2538,33 +2586,35 @@
     </row>
     <row r="130">
       <c r="B130" s="0" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C130" s="0" t="n">
         <v>140</v>
       </c>
       <c r="D130" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E130" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F130" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F130" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="131">
       <c r="B131" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C131" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D131" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E131" s="0" t="n">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="F131" s="0" t="inlineStr">
         <is>
@@ -2574,10 +2624,10 @@
     </row>
     <row r="132">
       <c r="B132" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C132" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -2587,16 +2637,16 @@
         </is>
       </c>
       <c r="B133" s="0" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C133" s="0" t="n">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="D133" s="0" t="n">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="E133" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="F133" s="0" t="inlineStr">
         <is>
@@ -2606,33 +2656,35 @@
     </row>
     <row r="134">
       <c r="B134" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C134" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D134" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E134" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F134" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F134" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="135">
       <c r="B135" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C135" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D135" s="0" t="n">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="E135" s="0" t="n">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="F135" s="0" t="inlineStr">
         <is>
@@ -2642,10 +2694,10 @@
     </row>
     <row r="136">
       <c r="B136" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C136" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -2655,16 +2707,16 @@
         </is>
       </c>
       <c r="B137" s="0" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C137" s="0" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="D137" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="E137" s="0" t="n">
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F137" s="0" t="inlineStr">
         <is>
@@ -2674,46 +2726,48 @@
     </row>
     <row r="138">
       <c r="B138" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C138" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D138" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E138" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="F138" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F138" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="139">
       <c r="B139" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C139" s="0" t="n">
         <v>30</v>
-      </c>
-      <c r="C139" s="0" t="n">
-        <v>120</v>
       </c>
       <c r="D139" s="0" t="n">
         <v>400</v>
       </c>
       <c r="E139" s="0" t="n">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="F139" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="B140" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.5019936597575131</v>
       </c>
       <c r="C140" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -2723,52 +2777,52 @@
         </is>
       </c>
       <c r="B141" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C141" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D141" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E141" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F141" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>500</v>
+      </c>
+      <c r="F141" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="142">
       <c r="B142" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C142" s="0" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="D142" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E142" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F142" s="0" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="F142" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="143">
       <c r="B143" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C143" s="0" t="n">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D143" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E143" s="0" t="n">
-        <v>1500</v>
+        <v>650</v>
       </c>
       <c r="F143" s="0" t="inlineStr">
         <is>
@@ -2778,10 +2832,10 @@
     </row>
     <row r="144">
       <c r="B144" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.7835120009355161</v>
       </c>
       <c r="C144" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -2791,65 +2845,65 @@
         </is>
       </c>
       <c r="B145" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C145" s="0" t="n">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D145" s="0" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E145" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F145" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>650</v>
+      </c>
+      <c r="F145" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" s="0" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C146" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D146" s="0" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E146" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="F146" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F146" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="147">
       <c r="B147" s="0" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C147" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D147" s="0" t="n">
         <v>400</v>
       </c>
       <c r="E147" s="0" t="n">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="F147" s="0" t="inlineStr">
         <is>
-          <t>3month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="B148" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.7835120009355161</v>
       </c>
       <c r="C148" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -2859,38 +2913,38 @@
         </is>
       </c>
       <c r="B149" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C149" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D149" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E149" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="F149" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>500</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C150" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D150" s="0" t="n">
-        <v>200</v>
+        <v>700</v>
       </c>
       <c r="E150" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F150" s="0" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="F150" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="151">
@@ -2898,13 +2952,13 @@
         <v>10</v>
       </c>
       <c r="C151" s="0" t="n">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="D151" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E151" s="0" t="n">
-        <v>1500</v>
+        <v>650</v>
       </c>
       <c r="F151" s="0" t="inlineStr">
         <is>
@@ -2914,10 +2968,10 @@
     </row>
     <row r="152">
       <c r="B152" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.7835120009355161</v>
       </c>
       <c r="C152" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -2927,52 +2981,52 @@
         </is>
       </c>
       <c r="B153" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C153" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D153" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E153" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F153" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>500</v>
+      </c>
+      <c r="F153" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C154" s="0" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="D154" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E154" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F154" s="0" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="F154" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="155">
       <c r="B155" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C155" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D155" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E155" s="0" t="n">
-        <v>1500</v>
+        <v>650</v>
       </c>
       <c r="F155" s="0" t="inlineStr">
         <is>
@@ -2982,10 +3036,10 @@
     </row>
     <row r="156">
       <c r="B156" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.7835120009355161</v>
       </c>
       <c r="C156" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -2995,52 +3049,52 @@
         </is>
       </c>
       <c r="B157" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C157" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D157" s="0" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="E157" s="0" t="n">
         <v>650</v>
       </c>
-      <c r="F157" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+      <c r="F157" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C158" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D158" s="0" t="n">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="E158" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F158" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F158" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="159">
       <c r="B159" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C159" s="0" t="n">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D159" s="0" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="E159" s="0" t="n">
-        <v>1500</v>
+        <v>650</v>
       </c>
       <c r="F159" s="0" t="inlineStr">
         <is>
@@ -3050,10 +3104,10 @@
     </row>
     <row r="160">
       <c r="B160" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.7835120009355161</v>
       </c>
       <c r="C160" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -3063,52 +3117,52 @@
         </is>
       </c>
       <c r="B161" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C161" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D161" s="0" t="n">
-        <v>550</v>
+        <v>0</v>
       </c>
       <c r="E161" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F161" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>650</v>
+      </c>
+      <c r="F161" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="162">
       <c r="B162" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C162" s="0" t="n">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D162" s="0" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E162" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="F162" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F162" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="163">
       <c r="B163" s="0" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C163" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D163" s="0" t="n">
-        <v>550</v>
+        <v>400</v>
       </c>
       <c r="E163" s="0" t="n">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="F163" s="0" t="inlineStr">
         <is>
@@ -3118,10 +3172,10 @@
     </row>
     <row r="164">
       <c r="B164" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-0.7835120009355161</v>
       </c>
       <c r="C164" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -3134,60 +3188,62 @@
         <v>10</v>
       </c>
       <c r="C165" s="0" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D165" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E165" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="F165" s="0" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="166">
       <c r="B166" s="0" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C166" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D166" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E166" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F166" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F166" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="167">
       <c r="B167" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C167" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D167" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E167" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F167" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="B168" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.036810723444095</v>
       </c>
       <c r="C168" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -3197,52 +3253,52 @@
         </is>
       </c>
       <c r="B169" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C169" s="0" t="n">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="D169" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E169" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="F169" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>700</v>
+      </c>
+      <c r="F169" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="170">
       <c r="B170" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C170" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D170" s="0" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E170" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F170" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F170" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="171">
       <c r="B171" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C171" s="0" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="D171" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E171" s="0" t="n">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="F171" s="0" t="inlineStr">
         <is>
@@ -3252,10 +3308,10 @@
     </row>
     <row r="172">
       <c r="B172" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.036810723444095</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
@@ -3268,60 +3324,62 @@
         <v>10</v>
       </c>
       <c r="C173" s="0" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D173" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E173" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="F173" s="0" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="174">
       <c r="B174" s="0" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C174" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D174" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E174" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F174" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F174" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="175">
       <c r="B175" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C175" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D175" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E175" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F175" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="B176" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.036810723444095</v>
       </c>
       <c r="C176" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -3331,52 +3389,52 @@
         </is>
       </c>
       <c r="B177" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C177" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="C177" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="D177" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E177" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F177" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>700</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="178">
       <c r="B178" s="0" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C178" s="0" t="n">
         <v>140</v>
       </c>
       <c r="D178" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E178" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F178" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F178" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="179">
       <c r="B179" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C179" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D179" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E179" s="0" t="n">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="F179" s="0" t="inlineStr">
         <is>
@@ -3386,10 +3444,10 @@
     </row>
     <row r="180">
       <c r="B180" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.036810723444095</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181">
@@ -3399,52 +3457,52 @@
         </is>
       </c>
       <c r="B181" s="0" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="D181" s="0" t="n">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="E181" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F181" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>700</v>
+      </c>
+      <c r="F181" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="182">
       <c r="B182" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C182" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D182" s="0" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E182" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="F182" s="0" t="n">
-        <v>5</v>
+        <v>700</v>
+      </c>
+      <c r="F182" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="183">
       <c r="B183" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C183" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D183" s="0" t="n">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="E183" s="0" t="n">
-        <v>750</v>
+        <v>600</v>
       </c>
       <c r="F183" s="0" t="inlineStr">
         <is>
@@ -3454,10 +3512,10 @@
     </row>
     <row r="184">
       <c r="B184" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.036810723444095</v>
       </c>
       <c r="C184" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -3467,63 +3525,65 @@
         </is>
       </c>
       <c r="B185" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D185" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E185" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="E185" s="0" t="n">
-        <v>600</v>
-      </c>
       <c r="F185" s="0" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="186">
       <c r="B186" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C186" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D186" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E186" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F186" s="0" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="F186" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="187">
       <c r="B187" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C187" s="0" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D187" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E187" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="F187" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="B188" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.116194832193996</v>
       </c>
       <c r="C188" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -3533,63 +3593,65 @@
         </is>
       </c>
       <c r="B189" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C189" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D189" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E189" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="E189" s="0" t="n">
-        <v>600</v>
-      </c>
       <c r="F189" s="0" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="190">
       <c r="B190" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C190" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D190" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E190" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F190" s="0" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="F190" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="191">
       <c r="B191" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C191" s="0" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D191" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E191" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="F191" s="0" t="inlineStr">
         <is>
-          <t>12month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="B192" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.116194832193996</v>
       </c>
       <c r="C192" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -3599,52 +3661,52 @@
         </is>
       </c>
       <c r="B193" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C193" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="D193" s="0" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E193" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F193" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>500</v>
+      </c>
+      <c r="F193" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="194">
       <c r="B194" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C194" s="0" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="D194" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E194" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="F194" s="0" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="F194" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="195">
       <c r="B195" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C195" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D195" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E195" s="0" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="F195" s="0" t="inlineStr">
         <is>
@@ -3654,10 +3716,10 @@
     </row>
     <row r="196">
       <c r="B196" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.116194832193996</v>
       </c>
       <c r="C196" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -3667,65 +3729,65 @@
         </is>
       </c>
       <c r="B197" s="0" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C197" s="0" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D197" s="0" t="n">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="E197" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F197" s="0" t="inlineStr">
-        <is>
-          <t>NOT ADAPTED</t>
-        </is>
+        <v>500</v>
+      </c>
+      <c r="F197" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="198">
       <c r="B198" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C198" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="D198" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E198" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="F198" s="0" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="F198" s="0" t="inlineStr">
+        <is>
+          <t>NOT ADAPTED</t>
+        </is>
       </c>
     </row>
     <row r="199">
       <c r="B199" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C199" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D199" s="0" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E199" s="0" t="n">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="F199" s="0" t="inlineStr">
         <is>
-          <t>6month charter</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="B200" s="0" t="n">
-        <v>0.2261956906511167</v>
+        <v>-1.116194832193996</v>
       </c>
       <c r="C200" s="0" t="n">
-        <v>0.006985778384696833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201">

</xml_diff>

<commit_message>
Implement charter in pattern.
</commit_message>
<xml_diff>
--- a/output/ship_rule_integrate.xlsx
+++ b/output/ship_rule_integrate.xlsx
@@ -383,22 +383,22 @@
         </is>
       </c>
       <c r="B1" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F1" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G1" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H1" s="0" t="inlineStr">
         <is>
@@ -408,22 +408,22 @@
     </row>
     <row r="2">
       <c r="B2" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
@@ -433,35 +433,35 @@
     </row>
     <row r="3">
       <c r="B3" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="H3" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>12month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.1793263158819565</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.1044080141801092</v>
       </c>
     </row>
     <row r="5">
@@ -471,22 +471,22 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H5" s="0" t="inlineStr">
         <is>
@@ -496,22 +496,22 @@
     </row>
     <row r="6">
       <c r="B6" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
@@ -521,35 +521,35 @@
     </row>
     <row r="7">
       <c r="B7" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="H7" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>12month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.1793263158819565</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.1044080141801092</v>
       </c>
     </row>
     <row r="9">
@@ -559,22 +559,22 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H9" s="0" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
     </row>
     <row r="10">
       <c r="B10" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H10" s="0" t="inlineStr">
         <is>
@@ -609,35 +609,35 @@
     </row>
     <row r="11">
       <c r="B11" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>12month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.1793263158819565</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.1044080141801092</v>
       </c>
     </row>
     <row r="13">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H13" s="0" t="inlineStr">
         <is>
@@ -672,22 +672,22 @@
     </row>
     <row r="14">
       <c r="B14" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="H14" s="0" t="inlineStr">
         <is>
@@ -697,35 +697,35 @@
     </row>
     <row r="15">
       <c r="B15" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>12month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.1793263158819565</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.1044080141801092</v>
       </c>
     </row>
     <row r="17">
@@ -735,22 +735,22 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H17" s="0" t="inlineStr">
         <is>
@@ -760,22 +760,22 @@
     </row>
     <row r="18">
       <c r="B18" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="H18" s="0" t="inlineStr">
         <is>
@@ -785,35 +785,35 @@
     </row>
     <row r="19">
       <c r="B19" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="H19" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>12month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.1793263158819565</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.1044080141801092</v>
       </c>
     </row>
     <row r="21">
@@ -823,22 +823,22 @@
         </is>
       </c>
       <c r="B21" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H21" s="0" t="inlineStr">
         <is>
@@ -848,22 +848,22 @@
     </row>
     <row r="22">
       <c r="B22" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="H22" s="0" t="inlineStr">
         <is>
@@ -873,35 +873,35 @@
     </row>
     <row r="23">
       <c r="B23" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="H23" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>12month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.1793263158819565</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.1044080141801092</v>
       </c>
     </row>
     <row r="25">
@@ -911,22 +911,22 @@
         </is>
       </c>
       <c r="B25" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H25" s="0" t="inlineStr">
         <is>
@@ -936,22 +936,22 @@
     </row>
     <row r="26">
       <c r="B26" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="H26" s="0" t="inlineStr">
         <is>
@@ -961,35 +961,35 @@
     </row>
     <row r="27">
       <c r="B27" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="H27" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>12month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.1793263158819565</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.1044080141801092</v>
       </c>
     </row>
     <row r="29">
@@ -999,22 +999,22 @@
         </is>
       </c>
       <c r="B29" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="H29" s="0" t="inlineStr">
         <is>
@@ -1024,22 +1024,22 @@
     </row>
     <row r="30">
       <c r="B30" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="H30" s="0" t="inlineStr">
         <is>
@@ -1049,35 +1049,35 @@
     </row>
     <row r="31">
       <c r="B31" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="H31" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>12month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.1793263158819565</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.1044080141801092</v>
       </c>
     </row>
     <row r="33">
@@ -1093,13 +1093,13 @@
         <v>140</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>1400</v>
+        <v>600</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>1800</v>
+        <v>900</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>110</v>
@@ -1112,60 +1112,60 @@
     </row>
     <row r="34">
       <c r="B34" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H34" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 50 ships</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C35" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C35" s="0" t="n">
-        <v>70</v>
-      </c>
       <c r="D35" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="H35" s="0" t="inlineStr">
         <is>
-          <t>12month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="0" t="n">
-        <v>0.3863699174990837</v>
+        <v>0.0751977170525911</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>0.2114099581093005</v>
+        <v>0.0007721638932780874</v>
       </c>
     </row>
     <row r="37">
@@ -1175,22 +1175,22 @@
         </is>
       </c>
       <c r="B37" s="0" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>1300</v>
+        <v>1800</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="H37" s="0" t="inlineStr">
         <is>
@@ -1200,60 +1200,60 @@
     </row>
     <row r="38">
       <c r="B38" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="H38" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 80 ships</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="0" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>1200</v>
+        <v>3000</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H39" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>3month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="0" t="n">
-        <v>0.4028644417949471</v>
+        <v>0.06551251724129391</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>0.3098197354549286</v>
+        <v>0.0009532033421444357</v>
       </c>
     </row>
     <row r="41">
@@ -1263,22 +1263,22 @@
         </is>
       </c>
       <c r="B41" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>1300</v>
+        <v>900</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="H41" s="0" t="inlineStr">
         <is>
@@ -1288,60 +1288,60 @@
     </row>
     <row r="42">
       <c r="B42" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D42" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E42" s="0" t="n">
         <v>800</v>
       </c>
-      <c r="E42" s="0" t="n">
-        <v>1200</v>
-      </c>
       <c r="F42" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="G42" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="G42" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="H42" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 25 ships</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="0" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>1200</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="H43" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>6month charter, 100 ships</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="0" t="n">
-        <v>0.4028644417949471</v>
+        <v>0.04709753181522083</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>0.3098197354549286</v>
+        <v>0.001777595180316166</v>
       </c>
     </row>
     <row r="45">
@@ -1351,22 +1351,22 @@
         </is>
       </c>
       <c r="B45" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="H45" s="0" t="inlineStr">
         <is>
@@ -1376,60 +1376,60 @@
     </row>
     <row r="46">
       <c r="B46" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>40</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>1200</v>
+        <v>3000</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="H46" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="H47" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>6month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="0" t="n">
-        <v>0.4028644417949471</v>
+        <v>0.008059392659000963</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>0.3098197354549286</v>
+        <v>0.09771099625629363</v>
       </c>
     </row>
     <row r="49">
@@ -1439,85 +1439,85 @@
         </is>
       </c>
       <c r="B49" s="0" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C49" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G49" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D49" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="G49" s="0" t="n">
-        <v>140</v>
-      </c>
       <c r="H49" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 12</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="H50" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 80 ships</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="0" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>1200</v>
+        <v>3000</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H51" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>6month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="0" t="n">
-        <v>0.4028644417949471</v>
+        <v>-0.03043678262807633</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>0.3098197354549286</v>
+        <v>0.001051820498873746</v>
       </c>
     </row>
     <row r="53">
@@ -1527,13 +1527,13 @@
         </is>
       </c>
       <c r="B53" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>1300</v>
@@ -1542,7 +1542,7 @@
         <v>50</v>
       </c>
       <c r="G53" s="0" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H53" s="0" t="inlineStr">
         <is>
@@ -1552,60 +1552,60 @@
     </row>
     <row r="54">
       <c r="B54" s="0" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>800</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="F54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="G54" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="H54" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 90 ships</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>140</v>
+        <v>50</v>
       </c>
       <c r="G55" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="H55" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="0" t="n">
-        <v>0.4028154862318819</v>
+        <v>-0.06502812508640564</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>0.309884376297173</v>
+        <v>0.0002856113359384135</v>
       </c>
     </row>
     <row r="57">
@@ -1615,85 +1615,85 @@
         </is>
       </c>
       <c r="B57" s="0" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="H57" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 14</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="G58" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H58" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 90 ships</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="B59" s="0" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G59" s="0" t="n">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="H59" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>36month charter, 1 ships</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="B60" s="0" t="n">
-        <v>0.3536974850635795</v>
+        <v>-0.07426429082354349</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>0.2733389254862325</v>
+        <v>0.0002285815737254787</v>
       </c>
     </row>
     <row r="61">
@@ -1703,85 +1703,85 @@
         </is>
       </c>
       <c r="B61" s="0" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="G61" s="0" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="H61" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 14</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="B62" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="G62" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H62" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 90 ships</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="B63" s="0" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G63" s="0" t="n">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="H63" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>36month charter, 1 ships</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="B64" s="0" t="n">
-        <v>0.3536974850635795</v>
+        <v>-0.07426429082354349</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>0.2733389254862325</v>
+        <v>0.0002285815737254787</v>
       </c>
     </row>
     <row r="65">
@@ -1791,22 +1791,22 @@
         </is>
       </c>
       <c r="B65" s="0" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C65" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="G65" s="0" t="n">
         <v>150</v>
-      </c>
-      <c r="D65" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E65" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F65" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="G65" s="0" t="n">
-        <v>140</v>
       </c>
       <c r="H65" s="0" t="inlineStr">
         <is>
@@ -1816,60 +1816,60 @@
     </row>
     <row r="66">
       <c r="B66" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>70</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="G66" s="0" t="n">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="H66" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 70 ships</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="B67" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>1200</v>
+        <v>3000</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H67" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>6month charter, 3 ships</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="B68" s="0" t="n">
-        <v>0.3536974850635795</v>
+        <v>-0.07605370193622697</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>0.2733389254862325</v>
+        <v>0.000191277701006062</v>
       </c>
     </row>
     <row r="69">
@@ -1879,85 +1879,85 @@
         </is>
       </c>
       <c r="B69" s="0" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G69" s="0" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H69" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 23</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="B70" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C70" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F70" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D70" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="E70" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F70" s="0" t="n">
-        <v>120</v>
-      </c>
       <c r="G70" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="H70" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 80 ships</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="B71" s="0" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>500</v>
+        <v>1100</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="G71" s="0" t="n">
         <v>140</v>
       </c>
       <c r="H71" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="B72" s="0" t="n">
-        <v>0.3536974850635795</v>
+        <v>-0.07606106141069571</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>0.2733389254862325</v>
+        <v>0.0001986350642842516</v>
       </c>
     </row>
     <row r="73">
@@ -1967,19 +1967,19 @@
         </is>
       </c>
       <c r="B73" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G73" s="0" t="n">
         <v>95</v>
@@ -1992,22 +1992,22 @@
     </row>
     <row r="74">
       <c r="B74" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="G74" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H74" s="0" t="inlineStr">
         <is>
@@ -2017,35 +2017,35 @@
     </row>
     <row r="75">
       <c r="B75" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>1200</v>
+        <v>3000</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G75" s="0" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="H75" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 60 ships</t>
+          <t>12month charter, 40 ships</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="B76" s="0" t="n">
-        <v>0.2070867263613882</v>
+        <v>-0.1058092353905502</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>0.2775864736382336</v>
+        <v>0.06581535506042055</v>
       </c>
     </row>
     <row r="77">
@@ -2055,19 +2055,19 @@
         </is>
       </c>
       <c r="B77" s="0" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G77" s="0" t="n">
         <v>95</v>
@@ -2080,22 +2080,22 @@
     </row>
     <row r="78">
       <c r="B78" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E78" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="G78" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H78" s="0" t="inlineStr">
         <is>
@@ -2105,35 +2105,35 @@
     </row>
     <row r="79">
       <c r="B79" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>1200</v>
+        <v>3000</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G79" s="0" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="H79" s="0" t="inlineStr">
         <is>
-          <t>3month charter, 60 ships</t>
+          <t>12month charter, 40 ships</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="B80" s="0" t="n">
-        <v>0.2070867263613882</v>
+        <v>-0.1058092353905502</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>0.2775864736382336</v>
+        <v>0.06581535506042055</v>
       </c>
     </row>
     <row r="81">
@@ -2143,22 +2143,22 @@
         </is>
       </c>
       <c r="B81" s="0" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>600</v>
+        <v>1500</v>
       </c>
       <c r="F81" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G81" s="0" t="n">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="H81" s="0" t="inlineStr">
         <is>
@@ -2168,60 +2168,60 @@
     </row>
     <row r="82">
       <c r="B82" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E82" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="F82" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="G82" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="H82" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 40 ships</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="B83" s="0" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C83" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F83" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="D83" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="E83" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F83" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="G83" s="0" t="n">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="H83" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 60 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="B84" s="0" t="n">
-        <v>0.2054048786545229</v>
+        <v>-0.1616963964504246</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>0.2554491074479501</v>
+        <v>0.01421662031598252</v>
       </c>
     </row>
     <row r="85">
@@ -2231,22 +2231,22 @@
         </is>
       </c>
       <c r="B85" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>1300</v>
+        <v>900</v>
       </c>
       <c r="F85" s="0" t="n">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="G85" s="0" t="n">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="H85" s="0" t="inlineStr">
         <is>
@@ -2256,60 +2256,60 @@
     </row>
     <row r="86">
       <c r="B86" s="0" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E86" s="0" t="n">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="G86" s="0" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H86" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="B87" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="G87" s="0" t="n">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="H87" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>36month charter, 15 ships</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="B88" s="0" t="n">
-        <v>0.1055882378903716</v>
+        <v>-0.2700261897926339</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>0.2613844648606211</v>
+        <v>0.1028390497449367</v>
       </c>
     </row>
     <row r="89">
@@ -2319,22 +2319,22 @@
         </is>
       </c>
       <c r="B89" s="0" t="n">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="G89" s="0" t="n">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="H89" s="0" t="inlineStr">
         <is>
@@ -2344,60 +2344,60 @@
     </row>
     <row r="90">
       <c r="B90" s="0" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C90" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F90" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D90" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="E90" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F90" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="G90" s="0" t="n">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="H90" s="0" t="inlineStr">
         <is>
-          <t>sell 20 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="B91" s="0" t="n">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>300</v>
+        <v>1300</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>900</v>
+        <v>2000</v>
       </c>
       <c r="F91" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G91" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="H91" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="B92" s="0" t="n">
-        <v>0.03735420569544133</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>0.04412231132886889</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="93">
@@ -2407,22 +2407,22 @@
         </is>
       </c>
       <c r="B93" s="0" t="n">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="G93" s="0" t="n">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H93" s="0" t="inlineStr">
         <is>
@@ -2432,60 +2432,60 @@
     </row>
     <row r="94">
       <c r="B94" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="E94" s="0" t="n">
-        <v>3000</v>
+        <v>1400</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G94" s="0" t="n">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="H94" s="0" t="inlineStr">
         <is>
-          <t>sell 20 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="B95" s="0" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>300</v>
+        <v>1200</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G95" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="H95" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 10 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="B96" s="0" t="n">
-        <v>0.03735420569544133</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>0.04412231132886889</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="97">
@@ -2498,23 +2498,23 @@
         <v>10</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E97" s="0" t="n">
-        <v>1800</v>
+        <v>700</v>
       </c>
       <c r="F97" s="0" t="n">
         <v>70</v>
       </c>
       <c r="G97" s="0" t="n">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="H97" s="0" t="inlineStr">
         <is>
-          <t>change speed to 18</t>
+          <t>change speed to 19</t>
         </is>
       </c>
     </row>
@@ -2523,19 +2523,19 @@
         <v>100</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E98" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G98" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H98" s="0" t="inlineStr">
         <is>
@@ -2545,35 +2545,35 @@
     </row>
     <row r="99">
       <c r="B99" s="0" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D99" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E99" s="0" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G99" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="H99" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 90 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="B100" s="0" t="n">
-        <v>0.03140441618436061</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>0.2053855290175475</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="101">
@@ -2583,26 +2583,26 @@
         </is>
       </c>
       <c r="B101" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F101" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C101" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="D101" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="E101" s="0" t="n">
-        <v>1800</v>
-      </c>
-      <c r="F101" s="0" t="n">
+      <c r="G101" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="G101" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H101" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 18</t>
         </is>
       </c>
     </row>
@@ -2611,57 +2611,57 @@
         <v>10</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E102" s="0" t="n">
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G102" s="0" t="n">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="H102" s="0" t="inlineStr">
         <is>
-          <t>sell 20 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="B103" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E103" s="0" t="n">
-        <v>900</v>
+        <v>2000</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G103" s="0" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H103" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 60 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="B104" s="0" t="n">
-        <v>0.03012080073491956</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C104" s="0" t="n">
-        <v>0.06258796300488659</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="105">
@@ -2671,85 +2671,85 @@
         </is>
       </c>
       <c r="B105" s="0" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C105" s="0" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>160</v>
       </c>
       <c r="H105" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 19</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="B106" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C106" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D106" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E106" s="0" t="n">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="F106" s="0" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G106" s="0" t="n">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="H106" s="0" t="inlineStr">
         <is>
-          <t>sell 20 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="B107" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C107" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D107" s="0" t="n">
         <v>300</v>
       </c>
       <c r="E107" s="0" t="n">
-        <v>900</v>
+        <v>1800</v>
       </c>
       <c r="F107" s="0" t="n">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="G107" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="H107" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 60 ships</t>
+          <t>3month charter, 0 ships</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="B108" s="0" t="n">
-        <v>0.03012080073491956</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C108" s="0" t="n">
-        <v>0.06258796300488659</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="109">
@@ -2759,26 +2759,26 @@
         </is>
       </c>
       <c r="B109" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F109" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C109" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="D109" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="E109" s="0" t="n">
-        <v>1800</v>
-      </c>
-      <c r="F109" s="0" t="n">
+      <c r="G109" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="G109" s="0" t="n">
-        <v>160</v>
-      </c>
       <c r="H109" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 18</t>
         </is>
       </c>
     </row>
@@ -2787,57 +2787,57 @@
         <v>10</v>
       </c>
       <c r="C110" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D110" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E110" s="0" t="n">
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G110" s="0" t="n">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="H110" s="0" t="inlineStr">
         <is>
-          <t>sell 20 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="B111" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C111" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E111" s="0" t="n">
-        <v>900</v>
+        <v>2000</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G111" s="0" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H111" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 60 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="B112" s="0" t="n">
-        <v>0.03012080073491956</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>0.06258796300488659</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="113">
@@ -2847,85 +2847,85 @@
         </is>
       </c>
       <c r="B113" s="0" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C113" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D113" s="0" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E113" s="0" t="n">
-        <v>1800</v>
+        <v>600</v>
       </c>
       <c r="F113" s="0" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="G113" s="0" t="n">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="H113" s="0" t="inlineStr">
         <is>
-          <t>change speed to 18</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="B114" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C114" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="C114" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="D114" s="0" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E114" s="0" t="n">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="F114" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G114" s="0" t="n">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="H114" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>sell 0 ships</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="B115" s="0" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C115" s="0" t="n">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="E115" s="0" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="F115" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="G115" s="0" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H115" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 90 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="B116" s="0" t="n">
-        <v>0.01727526523144558</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C116" s="0" t="n">
-        <v>0.2178986403383891</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="117">
@@ -2935,22 +2935,22 @@
         </is>
       </c>
       <c r="B117" s="0" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C117" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>600</v>
+        <v>1500</v>
       </c>
       <c r="E117" s="0" t="n">
-        <v>1300</v>
+        <v>2000</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G117" s="0" t="n">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="H117" s="0" t="inlineStr">
         <is>
@@ -2960,26 +2960,26 @@
     </row>
     <row r="118">
       <c r="B118" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C118" s="0" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D118" s="0" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="E118" s="0" t="n">
-        <v>1100</v>
+        <v>3000</v>
       </c>
       <c r="F118" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="G118" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H118" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
@@ -2988,32 +2988,32 @@
         <v>60</v>
       </c>
       <c r="C119" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D119" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E119" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="E119" s="0" t="n">
-        <v>1200</v>
-      </c>
       <c r="F119" s="0" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="G119" s="0" t="n">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="H119" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="B120" s="0" t="n">
-        <v>0.01027519790628957</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C120" s="0" t="n">
-        <v>0.3070911783310507</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="121">
@@ -3023,51 +3023,51 @@
         </is>
       </c>
       <c r="B121" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="C121" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D121" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E121" s="0" t="n">
-        <v>1300</v>
+        <v>800</v>
       </c>
       <c r="F121" s="0" t="n">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="G121" s="0" t="n">
         <v>140</v>
       </c>
       <c r="H121" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 19</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="B122" s="0" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C122" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="D122" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="E122" s="0" t="n">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="G122" s="0" t="n">
         <v>130</v>
       </c>
       <c r="H122" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
@@ -3076,32 +3076,32 @@
         <v>70</v>
       </c>
       <c r="C123" s="0" t="n">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="D123" s="0" t="n">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="E123" s="0" t="n">
-        <v>1200</v>
+        <v>3000</v>
       </c>
       <c r="F123" s="0" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="G123" s="0" t="n">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="H123" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 5 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="B124" s="0" t="n">
-        <v>-0.002635110589222617</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C124" s="0" t="n">
-        <v>0.3173168590590394</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="125">
@@ -3111,72 +3111,72 @@
         </is>
       </c>
       <c r="B125" s="0" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C125" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D125" s="0" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="E125" s="0" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="F125" s="0" t="n">
         <v>60</v>
       </c>
       <c r="G125" s="0" t="n">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="H125" s="0" t="inlineStr">
         <is>
-          <t>change speed to 20</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="B126" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C126" s="0" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="D126" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E126" s="0" t="n">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="G126" s="0" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="H126" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="B127" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>90</v>
       </c>
       <c r="D127" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E127" s="0" t="n">
-        <v>1800</v>
+        <v>500</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G127" s="0" t="n">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="H127" s="0" t="inlineStr">
         <is>
@@ -3186,10 +3186,10 @@
     </row>
     <row r="128">
       <c r="B128" s="0" t="n">
-        <v>-0.006793848212650952</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C128" s="0" t="n">
-        <v>0.3490593377313477</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="129">
@@ -3199,22 +3199,22 @@
         </is>
       </c>
       <c r="B129" s="0" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="C129" s="0" t="n">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D129" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E129" s="0" t="n">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="G129" s="0" t="n">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="H129" s="0" t="inlineStr">
         <is>
@@ -3224,47 +3224,47 @@
     </row>
     <row r="130">
       <c r="B130" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C130" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D130" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E130" s="0" t="n">
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="G130" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H130" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="B131" s="0" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C131" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D131" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E131" s="0" t="n">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G131" s="0" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H131" s="0" t="inlineStr">
         <is>
@@ -3274,10 +3274,10 @@
     </row>
     <row r="132">
       <c r="B132" s="0" t="n">
-        <v>-0.01271996316290907</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C132" s="0" t="n">
-        <v>0.3149033083912188</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="133">
@@ -3290,69 +3290,69 @@
         <v>10</v>
       </c>
       <c r="C133" s="0" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D133" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E133" s="0" t="n">
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="G133" s="0" t="n">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="H133" s="0" t="inlineStr">
         <is>
-          <t>change speed to 19</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="B134" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C134" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D134" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E134" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
       <c r="F134" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G134" s="0" t="n">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="H134" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 0 ships</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="B135" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C135" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D135" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E135" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F135" s="0" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="G135" s="0" t="n">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="H135" s="0" t="inlineStr">
         <is>
@@ -3362,10 +3362,10 @@
     </row>
     <row r="136">
       <c r="B136" s="0" t="n">
-        <v>-0.01271996316290907</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C136" s="0" t="n">
-        <v>0.3149033083912188</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="137">
@@ -3375,26 +3375,26 @@
         </is>
       </c>
       <c r="B137" s="0" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C137" s="0" t="n">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D137" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E137" s="0" t="n">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G137" s="0" t="n">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="H137" s="0" t="inlineStr">
         <is>
-          <t>change speed to 19</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
@@ -3406,41 +3406,41 @@
         <v>100</v>
       </c>
       <c r="D138" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="E138" s="0" t="n">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="F138" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G138" s="0" t="n">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="H138" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>sell 0 ships</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="B139" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C139" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D139" s="0" t="n">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="E139" s="0" t="n">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="F139" s="0" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="G139" s="0" t="n">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="H139" s="0" t="inlineStr">
         <is>
@@ -3450,10 +3450,10 @@
     </row>
     <row r="140">
       <c r="B140" s="0" t="n">
-        <v>-0.01271996316290907</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C140" s="0" t="n">
-        <v>0.3149033083912188</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="141">
@@ -3463,16 +3463,16 @@
         </is>
       </c>
       <c r="B141" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C141" s="0" t="n">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="D141" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E141" s="0" t="n">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="F141" s="0" t="n">
         <v>60</v>
@@ -3482,16 +3482,16 @@
       </c>
       <c r="H141" s="0" t="inlineStr">
         <is>
-          <t>change speed to 19</t>
+          <t>change speed to 18</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="B142" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C142" s="0" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D142" s="0" t="n">
         <v>500</v>
@@ -3500,35 +3500,35 @@
         <v>1800</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G142" s="0" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H142" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="B143" s="0" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C143" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D143" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E143" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="G143" s="0" t="n">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="H143" s="0" t="inlineStr">
         <is>
@@ -3538,10 +3538,10 @@
     </row>
     <row r="144">
       <c r="B144" s="0" t="n">
-        <v>-0.01271996316290907</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C144" s="0" t="n">
-        <v>0.3149033083912188</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="145">
@@ -3551,72 +3551,72 @@
         </is>
       </c>
       <c r="B145" s="0" t="n">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="C145" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D145" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E145" s="0" t="n">
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="F145" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G145" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H145" s="0" t="inlineStr">
         <is>
-          <t>change speed to 19</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="B146" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C146" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D146" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E146" s="0" t="n">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G146" s="0" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="H146" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="B147" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C147" s="0" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D147" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="E147" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F147" s="0" t="n">
         <v>50</v>
       </c>
       <c r="G147" s="0" t="n">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="H147" s="0" t="inlineStr">
         <is>
@@ -3626,10 +3626,10 @@
     </row>
     <row r="148">
       <c r="B148" s="0" t="n">
-        <v>-0.01271996316290907</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C148" s="0" t="n">
-        <v>0.3149033083912188</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="149">
@@ -3639,26 +3639,26 @@
         </is>
       </c>
       <c r="B149" s="0" t="n">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="C149" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D149" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E149" s="0" t="n">
-        <v>3000</v>
+        <v>800</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G149" s="0" t="n">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="H149" s="0" t="inlineStr">
         <is>
-          <t>change speed to 19</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
@@ -3667,44 +3667,44 @@
         <v>50</v>
       </c>
       <c r="C150" s="0" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D150" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E150" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G150" s="0" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H150" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="B151" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C151" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D151" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E151" s="0" t="n">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G151" s="0" t="n">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="H151" s="0" t="inlineStr">
         <is>
@@ -3714,10 +3714,10 @@
     </row>
     <row r="152">
       <c r="B152" s="0" t="n">
-        <v>-0.01271996316290907</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C152" s="0" t="n">
-        <v>0.3149033083912188</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="153">
@@ -3727,72 +3727,72 @@
         </is>
       </c>
       <c r="B153" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C153" s="0" t="n">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="D153" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E153" s="0" t="n">
-        <v>700</v>
+        <v>1200</v>
       </c>
       <c r="F153" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G153" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H153" s="0" t="inlineStr">
         <is>
-          <t>change speed to 19</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="B154" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C154" s="0" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D154" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E154" s="0" t="n">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="F154" s="0" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G154" s="0" t="n">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="H154" s="0" t="inlineStr">
         <is>
-          <t>sell 100 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="B155" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C155" s="0" t="n">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D155" s="0" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="E155" s="0" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="F155" s="0" t="n">
         <v>50</v>
       </c>
       <c r="G155" s="0" t="n">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="H155" s="0" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
     </row>
     <row r="156">
       <c r="B156" s="0" t="n">
-        <v>-0.01293369345524645</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C156" s="0" t="n">
-        <v>0.3299342049709236</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="157">
@@ -3815,47 +3815,47 @@
         </is>
       </c>
       <c r="B157" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C157" s="0" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="D157" s="0" t="n">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="E157" s="0" t="n">
         <v>1800</v>
       </c>
       <c r="F157" s="0" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G157" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H157" s="0" t="inlineStr">
         <is>
-          <t>change speed to 20</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="B158" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C158" s="0" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E158" s="0" t="n">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="F158" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G158" s="0" t="n">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="H158" s="0" t="inlineStr">
         <is>
@@ -3865,22 +3865,22 @@
     </row>
     <row r="159">
       <c r="B159" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C159" s="0" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D159" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E159" s="0" t="n">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="F159" s="0" t="n">
         <v>50</v>
       </c>
       <c r="G159" s="0" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H159" s="0" t="inlineStr">
         <is>
@@ -3890,10 +3890,10 @@
     </row>
     <row r="160">
       <c r="B160" s="0" t="n">
-        <v>-0.01546678947655049</v>
+        <v>-0.3195876800850752</v>
       </c>
       <c r="C160" s="0" t="n">
-        <v>0.335002991244646</v>
+        <v>0.08985452037021779</v>
       </c>
     </row>
     <row r="161">
@@ -3903,44 +3903,44 @@
         </is>
       </c>
       <c r="B161" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C161" s="0" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D161" s="0" t="n">
         <v>500</v>
       </c>
       <c r="E161" s="0" t="n">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="F161" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G161" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H161" s="0" t="inlineStr">
         <is>
-          <t>change speed to 20</t>
+          <t>change speed to 24</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="B162" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C162" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D162" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E162" s="0" t="n">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="F162" s="0" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G162" s="0" t="n">
         <v>95</v>
@@ -3953,22 +3953,22 @@
     </row>
     <row r="163">
       <c r="B163" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C163" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D163" s="0" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E163" s="0" t="n">
-        <v>1800</v>
+        <v>900</v>
       </c>
       <c r="F163" s="0" t="n">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="G163" s="0" t="n">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="H163" s="0" t="inlineStr">
         <is>
@@ -3978,10 +3978,10 @@
     </row>
     <row r="164">
       <c r="B164" s="0" t="n">
-        <v>-0.01546678947655049</v>
+        <v>-0.3199686243420975</v>
       </c>
       <c r="C164" s="0" t="n">
-        <v>0.335002991244646</v>
+        <v>0.08960606555915766</v>
       </c>
     </row>
     <row r="165">
@@ -3991,51 +3991,51 @@
         </is>
       </c>
       <c r="B165" s="0" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C165" s="0" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D165" s="0" t="n">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="E165" s="0" t="n">
-        <v>1800</v>
+        <v>600</v>
       </c>
       <c r="F165" s="0" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="G165" s="0" t="n">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="H165" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 24</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="B166" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C166" s="0" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D166" s="0" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E166" s="0" t="n">
         <v>3000</v>
       </c>
       <c r="F166" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="G166" s="0" t="n">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H166" s="0" t="inlineStr">
         <is>
-          <t>sell 20 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
@@ -4044,32 +4044,32 @@
         <v>10</v>
       </c>
       <c r="C167" s="0" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D167" s="0" t="n">
         <v>300</v>
       </c>
       <c r="E167" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="F167" s="0" t="n">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="G167" s="0" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="H167" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 60 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="B168" s="0" t="n">
-        <v>-0.01599536849338973</v>
+        <v>-0.3199686243420975</v>
       </c>
       <c r="C168" s="0" t="n">
-        <v>0.07071049251693109</v>
+        <v>0.08960606555915766</v>
       </c>
     </row>
     <row r="169">
@@ -4079,26 +4079,26 @@
         </is>
       </c>
       <c r="B169" s="0" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C169" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E169" s="0" t="n">
         <v>1200</v>
       </c>
-      <c r="E169" s="0" t="n">
-        <v>1800</v>
-      </c>
       <c r="F169" s="0" t="n">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="G169" s="0" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H169" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 14</t>
         </is>
       </c>
     </row>
@@ -4107,7 +4107,7 @@
         <v>10</v>
       </c>
       <c r="C170" s="0" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D170" s="0" t="n">
         <v>500</v>
@@ -4116,48 +4116,48 @@
         <v>3000</v>
       </c>
       <c r="F170" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="G170" s="0" t="n">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="H170" s="0" t="inlineStr">
         <is>
-          <t>sell 20 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="B171" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C171" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D171" s="0" t="n">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="E171" s="0" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="F171" s="0" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G171" s="0" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H171" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 60 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="B172" s="0" t="n">
-        <v>-0.01599536849338973</v>
+        <v>-0.4328540693605816</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>0.07071049251693109</v>
+        <v>0.04966479745970398</v>
       </c>
     </row>
     <row r="173">
@@ -4167,85 +4167,85 @@
         </is>
       </c>
       <c r="B173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D173" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="F173" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C173" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="D173" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="E173" s="0" t="n">
-        <v>1800</v>
-      </c>
-      <c r="F173" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="G173" s="0" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="H173" s="0" t="inlineStr">
         <is>
-          <t>NOT ADAPTED</t>
+          <t>change speed to 22</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="B174" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C174" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D174" s="0" t="n">
-        <v>500</v>
+        <v>1300</v>
       </c>
       <c r="E174" s="0" t="n">
         <v>3000</v>
       </c>
       <c r="F174" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G174" s="0" t="n">
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="H174" s="0" t="inlineStr">
         <is>
-          <t>sell 20 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="B175" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C175" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D175" s="0" t="n">
-        <v>300</v>
+        <v>800</v>
       </c>
       <c r="E175" s="0" t="n">
-        <v>800</v>
+        <v>1100</v>
       </c>
       <c r="F175" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G175" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="H175" s="0" t="inlineStr">
         <is>
-          <t>6month charter, 60 ships</t>
+          <t>NOT ADAPTED</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="B176" s="0" t="n">
-        <v>-0.01599536849338973</v>
+        <v>-0.4651637848562376</v>
       </c>
       <c r="C176" s="0" t="n">
-        <v>0.07071049251693109</v>
+        <v>0.1989874892748303</v>
       </c>
     </row>
     <row r="177">

</xml_diff>